<commit_message>
Added doors into bedroom in layout
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caden Wells\CSCI306\Clue\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caden Wells\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1024F06-A892-440C-9701-04B839173AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509774C-3180-4709-BFE7-01AA27FBCAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{158D1B4F-E646-48DC-B939-0EA967C9C0B0}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E35531-B35E-447A-8FB5-A2BD4DE38325}">
   <dimension ref="B1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2055,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="4" t="s">
         <v>1</v>
@@ -2689,7 +2689,7 @@
         <v>1</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Solved issue were all tests did not error when the tests package is run as a whole
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doggi\Desktop\eclipse\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caden Wells\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC81792D-E354-4DF2-A5C2-6A62B2A51896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761F518-7A3B-470F-B42C-E87015F537A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{158D1B4F-E646-48DC-B939-0EA967C9C0B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{158D1B4F-E646-48DC-B939-0EA967C9C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,94 +652,92 @@
   <dimension ref="B1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="1">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
       <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
       <c r="G1" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>6</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>8</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
-        <v>10</v>
-      </c>
       <c r="M1" s="1">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1">
         <v>11</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>12</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>13</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>14</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>15</v>
       </c>
-      <c r="R1" s="1">
-        <v>16</v>
-      </c>
       <c r="S1" s="1">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1">
         <v>17</v>
       </c>
-      <c r="T1" s="1">
-        <v>18</v>
-      </c>
       <c r="U1" s="1">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1">
         <v>19</v>
       </c>
-      <c r="V1" s="1">
+      <c r="W1" s="1">
         <v>20</v>
       </c>
-      <c r="W1" s="1">
+      <c r="X1" s="1">
         <v>21</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="1">
         <v>22</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Z1" s="1">
         <v>23</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AA1" s="1">
         <v>24</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
@@ -819,7 +817,7 @@
     </row>
     <row r="3" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -899,7 +897,7 @@
     </row>
     <row r="4" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -979,7 +977,7 @@
     </row>
     <row r="5" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -1059,7 +1057,7 @@
     </row>
     <row r="6" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
@@ -1139,7 +1137,7 @@
     </row>
     <row r="7" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
@@ -1219,7 +1217,7 @@
     </row>
     <row r="8" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>10</v>
@@ -1299,7 +1297,7 @@
     </row>
     <row r="9" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>10</v>
@@ -1379,7 +1377,7 @@
     </row>
     <row r="10" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>10</v>
@@ -1459,7 +1457,7 @@
     </row>
     <row r="11" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>10</v>
@@ -1539,7 +1537,7 @@
     </row>
     <row r="12" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
@@ -1619,7 +1617,7 @@
     </row>
     <row r="13" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>10</v>
@@ -1699,7 +1697,7 @@
     </row>
     <row r="14" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>10</v>
@@ -1779,7 +1777,7 @@
     </row>
     <row r="15" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>13</v>
@@ -1859,7 +1857,7 @@
     </row>
     <row r="16" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>10</v>
@@ -1939,7 +1937,7 @@
     </row>
     <row r="17" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -2019,7 +2017,7 @@
     </row>
     <row r="18" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>1</v>
@@ -2099,7 +2097,7 @@
     </row>
     <row r="19" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>1</v>
@@ -2179,7 +2177,7 @@
     </row>
     <row r="20" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>1</v>
@@ -2259,7 +2257,7 @@
     </row>
     <row r="21" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>1</v>
@@ -2339,7 +2337,7 @@
     </row>
     <row r="22" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>1</v>
@@ -2419,7 +2417,7 @@
     </row>
     <row r="23" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>1</v>
@@ -2499,7 +2497,7 @@
     </row>
     <row r="24" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>1</v>
@@ -2579,7 +2577,7 @@
     </row>
     <row r="25" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>1</v>
@@ -2659,7 +2657,7 @@
     </row>
     <row r="26" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Updated ClueLayout to display tests
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doggi\Desktop\eclipse\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC81792D-E354-4DF2-A5C2-6A62B2A51896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2A7A9F-54A1-4C4C-866E-A65940CE459C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{158D1B4F-E646-48DC-B939-0EA967C9C0B0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="46">
   <si>
     <t>T*</t>
   </si>
@@ -156,13 +156,31 @@
   </si>
   <si>
     <t>D#</t>
+  </si>
+  <si>
+    <t>Number of Doors: 17</t>
+  </si>
+  <si>
+    <t>Yellow: door direction test (in FileInitTests)</t>
+  </si>
+  <si>
+    <t>Light Orange: adjacency from rooms and doors</t>
+  </si>
+  <si>
+    <t>Dark Orange: adjacency walkways</t>
+  </si>
+  <si>
+    <t>Light Blue: Target tests</t>
+  </si>
+  <si>
+    <t>Turquoise: Test Occupied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +195,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +294,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF08DCD7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -282,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,6 +390,33 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,6 +425,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF08DCD7"/>
       <color rgb="FF990033"/>
       <color rgb="FFFF99FF"/>
     </mruColors>
@@ -649,15 +738,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E35531-B35E-447A-8FB5-A2BD4DE38325}">
-  <dimension ref="B1:AA26"/>
+  <dimension ref="B1:AC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="29" max="29" width="38.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -736,8 +828,11 @@
       <c r="AA1" s="1">
         <v>25</v>
       </c>
+      <c r="AC1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -750,7 +845,7 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -817,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -896,8 +991,11 @@
       <c r="AA3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="AC3" s="18" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -940,7 +1038,7 @@
       <c r="O4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="23" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="14" t="s">
@@ -976,8 +1074,11 @@
       <c r="AA4" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="AC4" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -987,7 +1088,7 @@
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1056,8 +1157,11 @@
       <c r="AA5" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="AC5" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -1067,7 +1171,7 @@
       <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1136,8 +1240,11 @@
       <c r="AA6" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="AC6" s="23" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="7" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -1162,7 +1269,7 @@
       <c r="I7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="26" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -1216,8 +1323,11 @@
       <c r="AA7" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="AC7" s="25" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="8" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -1248,7 +1358,7 @@
       <c r="K8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="17" t="s">
         <v>2</v>
       </c>
       <c r="M8" s="4" t="s">
@@ -1297,7 +1407,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>8</v>
       </c>
@@ -1316,7 +1426,7 @@
       <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="17" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -1377,7 +1487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>9</v>
       </c>
@@ -1396,7 +1506,7 @@
       <c r="G10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -1457,7 +1567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -1537,17 +1647,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="23" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -1598,7 +1708,7 @@
       <c r="U12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V12" s="4" t="s">
+      <c r="V12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="W12" s="4" t="s">
@@ -1617,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>12</v>
       </c>
@@ -1697,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>13</v>
       </c>
@@ -1752,7 +1862,7 @@
       <c r="S14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="T14" s="26" t="s">
         <v>1</v>
       </c>
       <c r="U14" s="4" t="s">
@@ -1777,7 +1887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>14</v>
       </c>
@@ -1857,7 +1967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:29" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>15</v>
       </c>
@@ -1974,7 +2084,7 @@
       <c r="M17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" s="23" t="s">
         <v>1</v>
       </c>
       <c r="O17" s="4" t="s">
@@ -2350,7 +2460,7 @@
       <c r="E22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="10" t="s">
@@ -2472,7 +2582,7 @@
       <c r="S23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="T23" s="17" t="s">
         <v>17</v>
       </c>
       <c r="U23" s="9" t="s">
@@ -2664,7 +2774,7 @@
       <c r="C26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="23" t="s">
         <v>1</v>
       </c>
       <c r="E26" s="4" t="s">

</xml_diff>